<commit_message>
Excel reader checkpoint; implemented named cell ranges --> subsets
</commit_message>
<xml_diff>
--- a/test/src/org/tms/io/sample2.xlsx
+++ b/test/src/org/tms/io/sample2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8900" yWindow="1320" windowWidth="20400" windowHeight="7200" tabRatio="500"/>
+    <workbookView xWindow="10560" yWindow="5900" windowWidth="14660" windowHeight="7440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sample 2" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="Booleans">'Sample 2'!$D:$D</definedName>
     <definedName name="Cyan">'Sample 2'!$C$5</definedName>
-    <definedName name="Subset">'Sample 2'!$B$2:$B$5</definedName>
+    <definedName name="Subset">'Sample 2'!$B$3:$D$5</definedName>
     <definedName name="YellowRow">'Sample 2'!$4:$4</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -585,7 +585,7 @@
       <c r="B2" s="1">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="b">
@@ -597,6 +597,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
+      <c r="C3" s="1"/>
       <c r="E3">
         <f>Table2[[#This Row],[Abc]]*3</f>
         <v>0</v>
@@ -606,7 +607,7 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="b">
@@ -624,7 +625,7 @@
       <c r="B5" s="1">
         <v>17.649999999999999</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="b">

</xml_diff>